<commit_message>
quick updates to MSFT and GOOG
</commit_message>
<xml_diff>
--- a/GOOG.xlsx
+++ b/GOOG.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26529"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26626"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\shkre\code\models\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{431D209B-B64B-4575-BC6F-36C5723B330E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A779EBF4-5334-406F-AB10-129945F1DF73}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="2700" yWindow="1290" windowWidth="31965" windowHeight="18945" xr2:uid="{605BC9F4-5436-4082-9BF9-F0067EF1EC53}"/>
+    <workbookView xWindow="-50145" yWindow="1845" windowWidth="23550" windowHeight="19425" activeTab="1" xr2:uid="{605BC9F4-5436-4082-9BF9-F0067EF1EC53}"/>
   </bookViews>
   <sheets>
     <sheet name="Main" sheetId="1" r:id="rId1"/>
@@ -805,14 +805,14 @@
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
   <xdr:twoCellAnchor>
     <xdr:from>
-      <xdr:col>19</xdr:col>
-      <xdr:colOff>31531</xdr:colOff>
+      <xdr:col>20</xdr:col>
+      <xdr:colOff>21505</xdr:colOff>
       <xdr:row>0</xdr:row>
       <xdr:rowOff>0</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>19</xdr:col>
-      <xdr:colOff>31531</xdr:colOff>
+      <xdr:col>20</xdr:col>
+      <xdr:colOff>21505</xdr:colOff>
       <xdr:row>109</xdr:row>
       <xdr:rowOff>76200</xdr:rowOff>
     </xdr:to>
@@ -829,8 +829,8 @@
       </xdr:nvCxnSpPr>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="11796548" y="0"/>
-          <a:ext cx="0" cy="17976631"/>
+          <a:off x="12414031" y="0"/>
+          <a:ext cx="0" cy="17562095"/>
         </a:xfrm>
         <a:prstGeom prst="line">
           <a:avLst/>
@@ -1228,8 +1228,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{32C51E30-7A56-49BA-9DA6-0CC9ECCB38E3}">
   <dimension ref="H1:N65"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="175" zoomScaleNormal="175" workbookViewId="0">
-      <selection activeCell="K24" sqref="K24"/>
+    <sheetView zoomScale="175" zoomScaleNormal="175" workbookViewId="0">
+      <selection activeCell="J10" sqref="J10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
@@ -1248,7 +1248,7 @@
         <v>0</v>
       </c>
       <c r="L2" s="1">
-        <v>105</v>
+        <v>131.33000000000001</v>
       </c>
     </row>
     <row r="3" spans="8:13" x14ac:dyDescent="0.2">
@@ -1271,7 +1271,7 @@
       </c>
       <c r="L4" s="3">
         <f>L2*L3</f>
-        <v>1359435</v>
+        <v>1700329.5100000002</v>
       </c>
     </row>
     <row r="5" spans="8:13" x14ac:dyDescent="0.2">
@@ -1303,7 +1303,7 @@
       </c>
       <c r="L7" s="3">
         <f>L4-L5+L6</f>
-        <v>1229882</v>
+        <v>1570776.5100000002</v>
       </c>
     </row>
     <row r="8" spans="8:13" x14ac:dyDescent="0.2">
@@ -1754,11 +1754,11 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{DFB0B16D-98AC-4F00-80A4-522691D39E31}">
   <dimension ref="A1:CW100"/>
   <sheetViews>
-    <sheetView zoomScale="145" zoomScaleNormal="145" workbookViewId="0">
-      <pane xSplit="2" ySplit="2" topLeftCell="L3" activePane="bottomRight" state="frozen"/>
+    <sheetView tabSelected="1" zoomScale="190" zoomScaleNormal="190" workbookViewId="0">
+      <pane xSplit="2" ySplit="2" topLeftCell="O3" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="C1" sqref="C1"/>
       <selection pane="bottomLeft" activeCell="A4" sqref="A4"/>
-      <selection pane="bottomRight" activeCell="P15" sqref="P15:S15"/>
+      <selection pane="bottomRight" activeCell="V18" sqref="V18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
@@ -1961,7 +1961,9 @@
       <c r="S3" s="11">
         <v>84</v>
       </c>
-      <c r="T3" s="11"/>
+      <c r="T3" s="11">
+        <v>3</v>
+      </c>
       <c r="U3" s="11"/>
       <c r="V3" s="11"/>
       <c r="AE3" s="3">
@@ -2036,11 +2038,10 @@
         <v>288</v>
       </c>
       <c r="T4" s="11">
-        <f t="shared" ref="T4:V4" si="4">+P4</f>
-        <v>193</v>
+        <v>285</v>
       </c>
       <c r="U4" s="11">
-        <f t="shared" si="4"/>
+        <f t="shared" ref="T4:V4" si="4">+Q4</f>
         <v>209</v>
       </c>
       <c r="V4" s="11">
@@ -2151,8 +2152,7 @@
         <v>7454</v>
       </c>
       <c r="T5" s="11">
-        <f>+P5*1.3</f>
-        <v>8158.8</v>
+        <v>8031</v>
       </c>
       <c r="U5" s="11">
         <f>+Q5*1.3</f>
@@ -2266,8 +2266,7 @@
         <v>7413</v>
       </c>
       <c r="T6" s="11">
-        <f>+P6*1.05</f>
-        <v>6880.6500000000005</v>
+        <v>8142</v>
       </c>
       <c r="U6" s="11">
         <f>+Q6*1.05</f>
@@ -2381,8 +2380,7 @@
         <v>7496</v>
       </c>
       <c r="T7" s="11">
-        <f>+P7*0.99</f>
-        <v>8176.41</v>
+        <v>7850</v>
       </c>
       <c r="U7" s="11">
         <f t="shared" ref="U7:V9" si="8">+Q7*1.03</f>
@@ -2496,8 +2494,7 @@
         <v>6693</v>
       </c>
       <c r="T8" s="11">
-        <f>+P8*0.99</f>
-        <v>7266.6</v>
+        <v>7665</v>
       </c>
       <c r="U8" s="11">
         <f t="shared" si="8"/>
@@ -2611,8 +2608,7 @@
         <v>40359</v>
       </c>
       <c r="T9" s="11">
-        <f>+P9*1.03</f>
-        <v>41909.67</v>
+        <v>42628</v>
       </c>
       <c r="U9" s="11">
         <f t="shared" si="8"/>
@@ -2749,7 +2745,7 @@
       </c>
       <c r="T10" s="11">
         <f>SUM(T6:T9)</f>
-        <v>64233.33</v>
+        <v>66285</v>
       </c>
       <c r="U10" s="11">
         <f>SUM(U6:U9)</f>
@@ -2889,7 +2885,7 @@
       </c>
       <c r="T11" s="10">
         <f t="shared" si="21"/>
-        <v>72585.13</v>
+        <v>74604</v>
       </c>
       <c r="U11" s="10">
         <f t="shared" si="21"/>
@@ -3025,7 +3021,7 @@
       </c>
       <c r="T12" s="11">
         <f t="shared" ref="T12:V12" si="31">T11*0.45</f>
-        <v>32663.308500000003</v>
+        <v>33571.800000000003</v>
       </c>
       <c r="U12" s="11">
         <f t="shared" si="31"/>
@@ -3200,7 +3196,7 @@
       </c>
       <c r="T14" s="11">
         <f t="shared" ref="T14:V14" si="37">T11-T12</f>
-        <v>39921.821500000005</v>
+        <v>41032.199999999997</v>
       </c>
       <c r="U14" s="11">
         <f t="shared" si="37"/>
@@ -3854,7 +3850,7 @@
       </c>
       <c r="T19" s="11">
         <f t="shared" si="66"/>
-        <v>19189.981500000005</v>
+        <v>20300.359999999997</v>
       </c>
       <c r="U19" s="11">
         <f t="shared" si="66"/>
@@ -4120,7 +4116,7 @@
       </c>
       <c r="T21" s="11">
         <f t="shared" si="79"/>
-        <v>18798.981500000005</v>
+        <v>19909.359999999997</v>
       </c>
       <c r="U21" s="11">
         <f t="shared" si="79"/>
@@ -4250,7 +4246,7 @@
       </c>
       <c r="T22" s="11">
         <f t="shared" ref="T22:V22" si="83">T21*0.2</f>
-        <v>3759.7963000000013</v>
+        <v>3981.8719999999994</v>
       </c>
       <c r="U22" s="11">
         <f t="shared" si="83"/>
@@ -4386,7 +4382,7 @@
       </c>
       <c r="T23" s="11">
         <f t="shared" si="91"/>
-        <v>15039.185200000004</v>
+        <v>15927.487999999998</v>
       </c>
       <c r="U23" s="11">
         <f t="shared" si="91"/>
@@ -4758,7 +4754,7 @@
       </c>
       <c r="T24" s="14">
         <f t="shared" si="102"/>
-        <v>1.1728289167901429</v>
+        <v>1.242103095999376</v>
       </c>
       <c r="U24" s="14">
         <f t="shared" si="102"/>
@@ -4973,7 +4969,7 @@
       </c>
       <c r="T27" s="16">
         <f t="shared" si="109"/>
-        <v>4.1617708258592234E-2</v>
+        <v>7.0589079428858392E-2</v>
       </c>
       <c r="U27" s="16">
         <f t="shared" si="109"/>
@@ -5089,7 +5085,9 @@
       <c r="S28" s="16">
         <v>0.06</v>
       </c>
-      <c r="T28" s="16"/>
+      <c r="T28" s="16">
+        <v>0.09</v>
+      </c>
       <c r="U28" s="16"/>
       <c r="V28" s="16"/>
       <c r="AJ28" s="18">
@@ -5152,7 +5150,7 @@
       </c>
       <c r="T29" s="15">
         <f t="shared" si="114"/>
-        <v>3.0000000000000027E-2</v>
+        <v>4.7654157143208309E-2</v>
       </c>
       <c r="U29" s="15">
         <f t="shared" si="114"/>
@@ -5271,7 +5269,7 @@
       </c>
       <c r="T30" s="15">
         <f t="shared" si="119"/>
-        <v>-9.9999999999998979E-3</v>
+        <v>4.4277929155313256E-2</v>
       </c>
       <c r="U30" s="15">
         <f t="shared" si="119"/>
@@ -5391,7 +5389,7 @@
       </c>
       <c r="T31" s="15">
         <f t="shared" si="127"/>
-        <v>2.2156394710459715E-2</v>
+        <v>5.4804984007256419E-2</v>
       </c>
       <c r="U31" s="15">
         <f t="shared" si="127"/>
@@ -5511,7 +5509,7 @@
       </c>
       <c r="T32" s="15">
         <f t="shared" si="135"/>
-        <v>0.30000000000000004</v>
+        <v>0.2796367112810707</v>
       </c>
       <c r="U32" s="15">
         <f t="shared" si="135"/>
@@ -5636,7 +5634,7 @@
       </c>
       <c r="T33" s="15">
         <f t="shared" si="143"/>
-        <v>0.55000000000000004</v>
+        <v>0.54999999999999993</v>
       </c>
       <c r="U33" s="15">
         <f t="shared" si="143"/>
@@ -5918,7 +5916,7 @@
       </c>
       <c r="T35" s="15">
         <f t="shared" si="163"/>
-        <v>0.57738644265016814</v>
+        <v>0.57139027397994746</v>
       </c>
       <c r="U35" s="15">
         <f t="shared" si="163"/>
@@ -6035,7 +6033,7 @@
       </c>
       <c r="T36" s="15">
         <f t="shared" si="168"/>
-        <v>0.79014365614554927</v>
+        <v>0.779354994370275</v>
       </c>
       <c r="U36" s="15">
         <f t="shared" si="168"/>
@@ -7881,7 +7879,9 @@
       <c r="S91" s="11">
         <v>190711</v>
       </c>
-      <c r="T91" s="11"/>
+      <c r="T91" s="11">
+        <v>181798</v>
+      </c>
       <c r="U91" s="11"/>
       <c r="V91" s="11"/>
     </row>
@@ -7908,6 +7908,10 @@
       <c r="S92" s="15">
         <f>+S91/O91-1</f>
         <v>0.16353885763791443</v>
+      </c>
+      <c r="T92" s="15">
+        <f>+T91/P91-1</f>
+        <v>4.4732033054811771E-2</v>
       </c>
     </row>
     <row r="93" spans="2:36" x14ac:dyDescent="0.2">

</xml_diff>